<commit_message>
try caching main list pages
</commit_message>
<xml_diff>
--- a/data/collection_schemas.xlsx
+++ b/data/collection_schemas.xlsx
@@ -166,7 +166,7 @@
     <t xml:space="preserve">Social housing</t>
   </si>
   <si>
-    <t xml:space="preserve">KO</t>
+    <t xml:space="preserve">HNZ</t>
   </si>
   <si>
     <t xml:space="preserve">hnz_clean</t>
@@ -676,11 +676,11 @@
   </sheetPr>
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C97" activeCellId="0" sqref="C97"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B60" activeCellId="0" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.57"/>

</xml_diff>